<commit_message>
added logo and 1 task
</commit_message>
<xml_diff>
--- a/monitoring.xlsx
+++ b/monitoring.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Schule\3Klasse\syp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Schule\3Klasse\syp\repositories\CHAT-PACK\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>server comm. Database</t>
+  </si>
+  <si>
+    <t>create logo</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,11 +480,11 @@
         <v>0.18</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D21" si="0">C3</f>
+        <f t="shared" ref="D3:D22" si="0">C3</f>
         <v>0.18</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E21" si="1">B3 - C3</f>
+        <f t="shared" ref="E3:E22" si="1">B3 - C3</f>
         <v>0.82000000000000006</v>
       </c>
     </row>
@@ -595,14 +598,8 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -712,14 +709,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -777,23 +768,36 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0.8</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4 A4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added gui, modi tasks
</commit_message>
<xml_diff>
--- a/monitoring.xlsx
+++ b/monitoring.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="oof">Sheet1!$D$24</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Task</t>
   </si>
@@ -87,6 +90,9 @@
   </si>
   <si>
     <t>set default picture</t>
+  </si>
+  <si>
+    <t>tb for each friend</t>
   </si>
 </sst>
 </file>
@@ -130,17 +136,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -437,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,12 +479,11 @@
         <v>0.18</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D23" si="0">C3</f>
         <v>0.18</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E23" si="1">B3 - C3</f>
-        <v>0.82000000000000006</v>
+        <f>C3 - D3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -502,12 +497,11 @@
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <f>B4 - C4</f>
-        <v>-1.5</v>
+        <f t="shared" ref="E4:E23" si="0">C4 - D4</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -521,11 +515,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="2"/>
@@ -533,12 +526,9 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -553,12 +543,11 @@
         <v>1.2</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -568,16 +557,15 @@
       <c r="B8">
         <v>0.25</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0.2</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>4.9999999999999989E-2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -587,22 +575,24 @@
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>0.5</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -615,12 +605,11 @@
         <v>2.5</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>-2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -631,15 +620,14 @@
         <v>0.75</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -652,13 +640,10 @@
       <c r="C13" s="1">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -672,23 +657,19 @@
         <v>5</v>
       </c>
       <c r="D14" s="1">
-        <f>C14</f>
         <v>5</v>
       </c>
       <c r="E14" s="1">
-        <f>B14 - C14</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -699,23 +680,22 @@
       <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -726,94 +706,116 @@
         <v>1.5</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1">
+        <v>3.32</v>
+      </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.32</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>32/60</f>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>0.8</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>0.3</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.25</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4 A4">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>